<commit_message>
update po dan pr
</commit_message>
<xml_diff>
--- a/public/doc/Format Impor Purchase Order.xlsx
+++ b/public/doc/Format Impor Purchase Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\mrp-new\public\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED007F3-1A4F-40BC-A635-A4E7BBDB8433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B7F5F2-9780-46F2-BEFA-DF3DF0338B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A62E235-4F2B-4897-B488-2903B036ACA3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Item Number</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Part name</t>
+  </si>
+  <si>
+    <t>Part number</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,8 +482,8 @@
     <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -515,10 +521,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>

</xml_diff>